<commit_message>
Added code on 05 june
</commit_message>
<xml_diff>
--- a/src/main/java/com/handelsgillet/testdata/HGAdminData.xlsx
+++ b/src/main/java/com/handelsgillet/testdata/HGAdminData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demo-master\src\main\java\com\handelsgillet\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7155" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="registrationData" sheetId="1" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="MemberLogin" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
   <si>
     <t>firstName</t>
   </si>
@@ -131,9 +127,6 @@
     <t>74984472374</t>
   </si>
   <si>
-    <t>w123</t>
-  </si>
-  <si>
     <t>560026</t>
   </si>
   <si>
@@ -143,51 +136,9 @@
     <t>Canada</t>
   </si>
   <si>
-    <t>event1</t>
-  </si>
-  <si>
-    <t>event2</t>
-  </si>
-  <si>
-    <t>notes1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>kumar 2</t>
-  </si>
-  <si>
-    <t>auto2</t>
-  </si>
-  <si>
-    <t>testing2</t>
-  </si>
-  <si>
     <t>abc2@gmail.com</t>
   </si>
   <si>
-    <t>TesterWorld2</t>
-  </si>
-  <si>
-    <t>Hindi2</t>
-  </si>
-  <si>
-    <t>English2</t>
-  </si>
-  <si>
-    <t>Hindi3</t>
-  </si>
-  <si>
-    <t>English3</t>
-  </si>
-  <si>
-    <t>Hindi4</t>
-  </si>
-  <si>
-    <t>English4</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -221,12 +172,6 @@
     <t>sdfdgdgggg</t>
   </si>
   <si>
-    <t>dgdgQa3</t>
-  </si>
-  <si>
-    <t>dggQa3</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -258,6 +203,126 @@
   </si>
   <si>
     <t>dfdQa</t>
+  </si>
+  <si>
+    <t>Testi</t>
+  </si>
+  <si>
+    <t>Testin</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>kuma</t>
+  </si>
+  <si>
+    <t>kumara</t>
+  </si>
+  <si>
+    <t>kumaaa</t>
+  </si>
+  <si>
+    <t>autooo</t>
+  </si>
+  <si>
+    <t>autoiii</t>
+  </si>
+  <si>
+    <t>autouuuu</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>japan</t>
+  </si>
+  <si>
+    <t>london</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>lead</t>
+  </si>
+  <si>
+    <t>architecture</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>TesterWo</t>
+  </si>
+  <si>
+    <t>TesterWor</t>
+  </si>
+  <si>
+    <t>dgdgQ</t>
+  </si>
+  <si>
+    <t>dgsgsgfs</t>
+  </si>
+  <si>
+    <t>dgdwgwg</t>
+  </si>
+  <si>
+    <t>dggsdg</t>
+  </si>
+  <si>
+    <t>sdgdsgg</t>
+  </si>
+  <si>
+    <t>gsdgsg</t>
+  </si>
+  <si>
+    <t>sdgsg</t>
+  </si>
+  <si>
+    <t>dgsgdgg</t>
+  </si>
+  <si>
+    <t>sdgsgsg</t>
+  </si>
+  <si>
+    <t>sgsgsgsg</t>
+  </si>
+  <si>
+    <t>sdgdhrhthfhfh</t>
+  </si>
+  <si>
+    <t>ggdgdgdgdggdg</t>
+  </si>
+  <si>
+    <t>gdgdgdg</t>
+  </si>
+  <si>
+    <t>gdgege</t>
+  </si>
+  <si>
+    <t>drhdhehdh</t>
+  </si>
+  <si>
+    <t>heheher</t>
+  </si>
+  <si>
+    <t>ghehe</t>
+  </si>
+  <si>
+    <t>workTitle</t>
+  </si>
+  <si>
+    <t>jjhfshsh</t>
+  </si>
+  <si>
+    <t>fdhsfdhfshsf</t>
+  </si>
+  <si>
+    <t>fhshh</t>
+  </si>
+  <si>
+    <t>fhdhdhd</t>
   </si>
 </sst>
 </file>
@@ -700,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -714,17 +779,17 @@
     <col min="7" max="8" width="14.42578125" style="1" customWidth="1"/>
     <col min="9" max="12" width="15.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" customWidth="1"/>
-    <col min="20" max="1020" width="14.42578125" customWidth="1"/>
-    <col min="1021" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="14" max="15" width="14.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" customWidth="1"/>
+    <col min="21" max="1021" width="14.42578125" customWidth="1"/>
+    <col min="1022" max="1026" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -767,49 +832,52 @@
       <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>25</v>
@@ -818,7 +886,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>27</v>
@@ -830,7 +898,7 @@
         <v>29</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>30</v>
@@ -839,63 +907,66 @@
         <v>31</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="U2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="X2" s="6" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="Y2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="D3" s="10">
         <v>42869</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>27</v>
@@ -904,10 +975,10 @@
         <v>28</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>30</v>
@@ -916,63 +987,66 @@
         <v>31</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="N3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="D4" s="10">
         <v>42869</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>27</v>
@@ -981,10 +1055,10 @@
         <v>28</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>30</v>
@@ -993,63 +1067,66 @@
         <v>31</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="N4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="O4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="D5" s="10">
         <v>42869</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>27</v>
@@ -1058,10 +1135,10 @@
         <v>28</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>30</v>
@@ -1070,43 +1147,46 @@
         <v>31</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="O5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="R5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="T5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="U5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="W5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="T5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="X5" s="6" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>40</v>
+        <v>91</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1137,18 +1217,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1177,18 +1257,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1220,15 +1300,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B2" s="11">
         <v>713912</v>

</xml_diff>

<commit_message>
Commited on 17 june 2018
</commit_message>
<xml_diff>
--- a/src/main/java/com/handelsgillet/testdata/HGAdminData.xlsx
+++ b/src/main/java/com/handelsgillet/testdata/HGAdminData.xlsx
@@ -3,17 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demo-master\src\main\java\com\handelsgillet\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7155" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19815" windowHeight="7155" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="registrationData" sheetId="1" r:id="rId1"/>
-    <sheet name="SuperAdminLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="ClubAdminLogin" sheetId="3" r:id="rId3"/>
-    <sheet name="MemberLogin" sheetId="4" r:id="rId4"/>
+    <sheet name="CreateTag" sheetId="5" r:id="rId2"/>
+    <sheet name="SuperAdminLogin" sheetId="2" r:id="rId3"/>
+    <sheet name="CreateEvent" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="ClubAdminLogin" sheetId="3" r:id="rId6"/>
+    <sheet name="MemberLogin" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -23,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
   <si>
     <t>firstName</t>
   </si>
@@ -323,6 +330,111 @@
   </si>
   <si>
     <t>fhdhdhd</t>
+  </si>
+  <si>
+    <t>Tag Name</t>
+  </si>
+  <si>
+    <t>Tag Description</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>This is description please enter all this in the text box as this we can see.</t>
+  </si>
+  <si>
+    <t>Event Name</t>
+  </si>
+  <si>
+    <t>Event Subject</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Strat Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Seats</t>
+  </si>
+  <si>
+    <t>Special Guest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Fees Per Person</t>
+  </si>
+  <si>
+    <t>Fees Description</t>
+  </si>
+  <si>
+    <t>Pool Part</t>
+  </si>
+  <si>
+    <t>Disco night</t>
+  </si>
+  <si>
+    <t>Comedy Night</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>Dance</t>
+  </si>
+  <si>
+    <t>Laughter</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Lomdon</t>
+  </si>
+  <si>
+    <t>John Cena</t>
+  </si>
+  <si>
+    <t>HHH</t>
+  </si>
+  <si>
+    <t>Byonce</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to </t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>enjoy</t>
+  </si>
+  <si>
+    <t>DJ</t>
   </si>
 </sst>
 </file>
@@ -386,7 +498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -416,6 +528,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -765,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -789,7 +903,7 @@
     <col min="1022" max="1026" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -869,7 +983,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>54</v>
       </c>
@@ -949,7 +1063,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
@@ -1029,7 +1143,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>61</v>
       </c>
@@ -1109,7 +1223,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
@@ -1205,6 +1319,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
@@ -1240,7 +1388,212 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="15">
+        <v>43273</v>
+      </c>
+      <c r="E2" s="15">
+        <v>43273</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="15">
+        <v>43314</v>
+      </c>
+      <c r="E1" s="15">
+        <v>43314</v>
+      </c>
+      <c r="F1" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G1" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H1">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="15">
+        <v>43292</v>
+      </c>
+      <c r="E2" s="15">
+        <v>43292</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1284,11 +1637,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>